<commit_message>
add amg chapter 2
</commit_message>
<xml_diff>
--- a/xjh/pictures/第一章/GPU加速的CFD应用.xlsx
+++ b/xjh/pictures/第一章/GPU加速的CFD应用.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xjh/thesis/xjh/pictures/第一章/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7275DC-78B3-EC41-9E15-71092505F00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE53A17-73D7-B143-A694-98A9C7A5505D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D007F42E-E5A1-4A4E-A7DD-78696C52F067}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>非结构化</t>
   </si>
@@ -43,12 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Altair AcuSolve</t>
-  </si>
-  <si>
-    <t>PACEFISH</t>
-  </si>
-  <si>
     <t>HIFUN</t>
   </si>
   <si>
@@ -129,6 +123,18 @@
   </si>
   <si>
     <t>叶轮机械URANS模拟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂几何外形的高升力流动问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通用CFD商业软件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA2541E-2040-5241-8D45-135B50302CB6}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -568,20 +574,20 @@
   <sheetData>
     <row r="1" spans="1:11" ht="55" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -591,16 +597,16 @@
     </row>
     <row r="2" spans="1:11" ht="156" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4"/>
@@ -614,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
@@ -625,16 +631,16 @@
     </row>
     <row r="4" spans="1:11" ht="25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="4"/>
@@ -647,45 +653,53 @@
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="24">
+    <row r="6" spans="1:11" ht="25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="25">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="24">
+    <row r="8" spans="1:11" ht="25">
       <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -694,20 +708,18 @@
     </row>
     <row r="9" spans="1:11" ht="24">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="24">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -749,27 +761,21 @@
       <c r="F13" s="4"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="24">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="24">
-      <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="2"/>
+    <row r="14" spans="1:11">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6"/>
@@ -787,25 +793,9 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="39" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
+    <row r="20" spans="1:6" ht="39" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>